<commit_message>
input soil moisture and bbch values
</commit_message>
<xml_diff>
--- a/data/treatmentC.xlsx
+++ b/data/treatmentC.xlsx
@@ -1,32 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/freezingexperiment/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="2920" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TX.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TX.csv!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TX.csv!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="211">
   <si>
     <t>OLD</t>
   </si>
@@ -373,9 +378,6 @@
     <t>ALNINC_S12</t>
   </si>
   <si>
-    <t>ALNINC_S13</t>
-  </si>
-  <si>
     <t>ALNINC_W14</t>
   </si>
   <si>
@@ -656,6 +658,12 @@
   </si>
   <si>
     <t>soil.11.Feb</t>
+  </si>
+  <si>
+    <t>BBCH.11.Feb</t>
+  </si>
+  <si>
+    <t>ALNINC_H13</t>
   </si>
 </sst>
 </file>
@@ -977,7 +985,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -985,20 +993,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,13 +1020,16 @@
         <v>86</v>
       </c>
       <c r="E1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" t="s">
         <v>209</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1028,8 +1039,11 @@
       <c r="C2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1039,8 +1053,11 @@
       <c r="C3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1050,8 +1067,11 @@
       <c r="C4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1061,8 +1081,11 @@
       <c r="C5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1072,8 +1095,11 @@
       <c r="C6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1083,8 +1109,11 @@
       <c r="C7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1094,8 +1123,11 @@
       <c r="C8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1105,8 +1137,11 @@
       <c r="C9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1116,8 +1151,11 @@
       <c r="C10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -1127,8 +1165,11 @@
       <c r="C11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -1138,8 +1179,11 @@
       <c r="C12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -1149,8 +1193,11 @@
       <c r="C13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1160,8 +1207,11 @@
       <c r="C14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1171,8 +1221,11 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1182,382 +1235,517 @@
       <c r="C16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="E16">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="E17">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="E19">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
         <v>131</v>
       </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" t="s">
-        <v>132</v>
-      </c>
       <c r="C22" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="E22">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="E23">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="E24">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
       <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25">
+        <v>7.8</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>140</v>
       </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>141</v>
       </c>
-      <c r="B26" t="s">
-        <v>142</v>
-      </c>
       <c r="C26" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="E26">
+        <v>7.3</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="E27">
+        <v>7.6</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C28" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="E28">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" t="s">
         <v>146</v>
       </c>
-      <c r="B29" t="s">
-        <v>147</v>
-      </c>
       <c r="C29" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="E29">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="E30">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="E31">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" t="s">
         <v>144</v>
       </c>
-      <c r="B32" t="s">
-        <v>145</v>
-      </c>
       <c r="C32" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="E32">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" t="s">
         <v>160</v>
       </c>
-      <c r="B33" t="s">
-        <v>161</v>
-      </c>
       <c r="C33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="E33">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>62</v>
       </c>
       <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>163</v>
       </c>
-      <c r="C34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>164</v>
       </c>
-      <c r="B35" t="s">
-        <v>165</v>
-      </c>
       <c r="C35" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="E35">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>62</v>
       </c>
       <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" t="s">
         <v>166</v>
       </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" t="s">
-        <v>167</v>
-      </c>
       <c r="C37" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="E37">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="E38">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="E39">
+        <v>8.9</v>
+      </c>
+      <c r="F39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="E40">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C41" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="E41">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="E42">
+        <v>8.4</v>
+      </c>
+      <c r="F42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C43" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="E43">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="E44">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C45" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="E45">
+        <v>9</v>
+      </c>
+      <c r="F45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" t="s">
         <v>179</v>
       </c>
-      <c r="B46" t="s">
-        <v>180</v>
-      </c>
       <c r="C46" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="E46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="E47">
+        <v>7.6</v>
+      </c>
+      <c r="F47">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
         <v>185</v>
       </c>
-      <c r="C48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>179</v>
-      </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
       <c r="C49" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="E49">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C50" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="E50">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1567,8 +1755,11 @@
       <c r="C51" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="E51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1578,8 +1769,11 @@
       <c r="C52" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="E52">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1589,8 +1783,11 @@
       <c r="C53" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="E53">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1600,8 +1797,11 @@
       <c r="C54" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="E54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -1611,8 +1811,11 @@
       <c r="C55" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="E55">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -1622,52 +1825,67 @@
       <c r="C56" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="E56">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C57" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="E57">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="E58">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="E59">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="E60">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -1677,426 +1895,573 @@
       <c r="C61" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="E61">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>210</v>
       </c>
       <c r="C62" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="E62">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="E63">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C64" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="E64">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="E65">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="E66">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C67" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="E67">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="E68">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="E69">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="E70">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C71" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="E71">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C72" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="E72">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>42</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C73" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="E73">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>44</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C74" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="E74">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>44</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C75" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="E75">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>44</v>
       </c>
       <c r="B76" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" t="s">
+        <v>92</v>
+      </c>
+      <c r="E76">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" t="s">
+        <v>151</v>
+      </c>
+      <c r="C77" t="s">
+        <v>92</v>
+      </c>
+      <c r="E77">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>145</v>
+      </c>
+      <c r="B78" t="s">
+        <v>153</v>
+      </c>
+      <c r="C78" t="s">
+        <v>92</v>
+      </c>
+      <c r="E78">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" t="s">
         <v>158</v>
       </c>
-      <c r="C76" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>151</v>
-      </c>
-      <c r="B77" t="s">
-        <v>152</v>
-      </c>
-      <c r="C77" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>146</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="C79" t="s">
+        <v>92</v>
+      </c>
+      <c r="E79">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" t="s">
         <v>154</v>
       </c>
-      <c r="C78" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>146</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
+      <c r="E80">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F80">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" t="s">
+        <v>156</v>
+      </c>
+      <c r="C81" t="s">
+        <v>92</v>
+      </c>
+      <c r="E81">
+        <v>11.1</v>
+      </c>
+      <c r="F81">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>159</v>
       </c>
-      <c r="C79" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>144</v>
-      </c>
-      <c r="B80" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>144</v>
-      </c>
-      <c r="B81" t="s">
-        <v>157</v>
-      </c>
-      <c r="C81" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>160</v>
-      </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C82" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="E82">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>58</v>
       </c>
       <c r="B83" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C83" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="E83">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>62</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C84" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="E84">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>62</v>
       </c>
       <c r="B85" t="s">
+        <v>169</v>
+      </c>
+      <c r="C85" t="s">
+        <v>92</v>
+      </c>
+      <c r="E85">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
         <v>170</v>
       </c>
-      <c r="C85" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
+      <c r="C86" t="s">
+        <v>92</v>
+      </c>
+      <c r="E86">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>172</v>
       </c>
-      <c r="B86" t="s">
-        <v>171</v>
-      </c>
-      <c r="C86" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+      <c r="B87" t="s">
         <v>173</v>
       </c>
-      <c r="B87" t="s">
-        <v>174</v>
-      </c>
       <c r="C87" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="E87">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>67</v>
       </c>
       <c r="B88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C88" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="E88">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>71</v>
       </c>
       <c r="B89" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" t="s">
+        <v>92</v>
+      </c>
+      <c r="E89">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>196</v>
       </c>
-      <c r="C89" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+      <c r="B90" t="s">
         <v>197</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>92</v>
+      </c>
+      <c r="E90">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F90">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>196</v>
+      </c>
+      <c r="B91" t="s">
         <v>198</v>
       </c>
-      <c r="C90" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>197</v>
-      </c>
-      <c r="B91" t="s">
-        <v>199</v>
-      </c>
       <c r="C91" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="E91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>79</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="E92">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F92">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>79</v>
       </c>
       <c r="B93" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="E93">
+        <v>8.1</v>
+      </c>
+      <c r="F93">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="E94">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F94">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>79</v>
       </c>
       <c r="B95" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C95" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="E95">
+        <v>9.6</v>
+      </c>
+      <c r="F95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C96" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <v>8.5</v>
+      </c>
+      <c r="F96">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>74</v>
       </c>
       <c r="B97" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C97" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>74</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C98" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98">
+        <v>9</v>
+      </c>
+      <c r="F98">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B99" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C99" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99">
+        <v>7.4</v>
+      </c>
+      <c r="F99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -2109,8 +2474,11 @@
       <c r="D100">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -2123,8 +2491,11 @@
       <c r="D101">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -2137,8 +2508,11 @@
       <c r="D102">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -2151,8 +2525,11 @@
       <c r="D103">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -2165,8 +2542,11 @@
       <c r="D104">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -2179,8 +2559,11 @@
       <c r="D105">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -2193,8 +2576,14 @@
       <c r="D106">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F106">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -2207,8 +2596,11 @@
       <c r="D107">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>13</v>
       </c>
@@ -2221,8 +2613,11 @@
       <c r="D108">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -2235,8 +2630,11 @@
       <c r="D109">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>29</v>
       </c>
@@ -2249,8 +2647,11 @@
       <c r="D110">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -2263,8 +2664,11 @@
       <c r="D111" s="1">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="E111">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -2277,8 +2681,11 @@
       <c r="D112">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -2291,8 +2698,11 @@
       <c r="D113">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>20</v>
       </c>
@@ -2305,8 +2715,11 @@
       <c r="D114">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>22</v>
       </c>
@@ -2319,8 +2732,11 @@
       <c r="D115">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>22</v>
       </c>
@@ -2333,8 +2749,11 @@
       <c r="D116">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>38</v>
       </c>
@@ -2347,8 +2766,11 @@
       <c r="D117">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>37</v>
       </c>
@@ -2361,8 +2783,11 @@
       <c r="D118">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>32</v>
       </c>
@@ -2375,8 +2800,11 @@
       <c r="D119">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>40</v>
       </c>
@@ -2389,8 +2817,11 @@
       <c r="D120">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>34</v>
       </c>
@@ -2403,8 +2834,11 @@
       <c r="D121">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="E121">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -2417,8 +2851,11 @@
       <c r="D122">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>44</v>
       </c>
@@ -2431,8 +2868,11 @@
       <c r="D123">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>44</v>
       </c>
@@ -2445,8 +2885,11 @@
       <c r="D124">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>44</v>
       </c>
@@ -2459,8 +2902,14 @@
       <c r="D125">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125">
+        <v>9.1</v>
+      </c>
+      <c r="F125">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>44</v>
       </c>
@@ -2473,8 +2922,14 @@
       <c r="D126">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126">
+        <v>7.7</v>
+      </c>
+      <c r="F126">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>50</v>
       </c>
@@ -2487,8 +2942,11 @@
       <c r="D127">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>50</v>
       </c>
@@ -2501,8 +2959,11 @@
       <c r="D128">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>53</v>
       </c>
@@ -2515,8 +2976,11 @@
       <c r="D129">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>46</v>
       </c>
@@ -2529,8 +2993,14 @@
       <c r="D130">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130">
+        <v>9.6</v>
+      </c>
+      <c r="F130">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>56</v>
       </c>
@@ -2543,8 +3013,11 @@
       <c r="D131">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>58</v>
       </c>
@@ -2557,8 +3030,11 @@
       <c r="D132">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>60</v>
       </c>
@@ -2571,8 +3047,11 @@
       <c r="D133">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>62</v>
       </c>
@@ -2585,8 +3064,11 @@
       <c r="D134">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>62</v>
       </c>
@@ -2599,8 +3081,11 @@
       <c r="D135">
         <v>10.1</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>64</v>
       </c>
@@ -2613,8 +3098,11 @@
       <c r="D136">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>67</v>
       </c>
@@ -2627,8 +3115,14 @@
       <c r="D137">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137">
+        <v>10.9</v>
+      </c>
+      <c r="F137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>71</v>
       </c>
@@ -2641,8 +3135,11 @@
       <c r="D138">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>67</v>
       </c>
@@ -2655,8 +3152,11 @@
       <c r="D139">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>71</v>
       </c>
@@ -2669,8 +3169,14 @@
       <c r="D140">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140">
+        <v>7.9</v>
+      </c>
+      <c r="F140">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>68</v>
       </c>
@@ -2683,8 +3189,14 @@
       <c r="D141">
         <v>10.7</v>
       </c>
-    </row>
-    <row r="142" spans="1:4">
+      <c r="E141">
+        <v>9.1</v>
+      </c>
+      <c r="F141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>77</v>
       </c>
@@ -2697,8 +3209,11 @@
       <c r="D142">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>79</v>
       </c>
@@ -2711,8 +3226,11 @@
       <c r="D143">
         <v>8</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>74</v>
       </c>
@@ -2725,8 +3243,11 @@
       <c r="D144">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>74</v>
       </c>
@@ -2739,8 +3260,11 @@
       <c r="D145">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>74</v>
       </c>
@@ -2753,8 +3277,11 @@
       <c r="D146">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="E146">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>74</v>
       </c>
@@ -2767,8 +3294,14 @@
       <c r="D147">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="E147">
+        <v>7.3</v>
+      </c>
+      <c r="F147">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>84</v>
       </c>
@@ -2781,9 +3314,15 @@
       <c r="D148">
         <v>7.7</v>
       </c>
+      <c r="E148">
+        <v>8.1</v>
+      </c>
+      <c r="F148">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
+  <autoFilter ref="A1:G1">
     <sortState ref="A2:F148">
       <sortCondition ref="C1:C148"/>
     </sortState>
@@ -2792,11 +3331,6 @@
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2808,32 +3342,32 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>203</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>206</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>207</v>
       </c>
-      <c r="G1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42766</v>
       </c>
@@ -2856,7 +3390,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42777</v>
       </c>
@@ -2881,10 +3415,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new information to data
</commit_message>
<xml_diff>
--- a/data/treatmentC.xlsx
+++ b/data/treatmentC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="3620" windowWidth="36680" windowHeight="22120" tabRatio="500"/>
+    <workbookView xWindow="12560" yWindow="3620" windowWidth="36680" windowHeight="22120" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="GH" sheetId="2" r:id="rId3"/>
     <sheet name="FRZ" sheetId="3" r:id="rId4"/>
     <sheet name="tx.counts" sheetId="5" r:id="rId5"/>
+    <sheet name="soil.moisture" sheetId="7" r:id="rId6"/>
+    <sheet name="monitor" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">FRZ!$A$1:$G$1</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="257">
   <si>
     <t>OLD</t>
   </si>
@@ -770,6 +772,42 @@
   </si>
   <si>
     <t>Do again with cuttings!!</t>
+  </si>
+  <si>
+    <t>boat.wt</t>
+  </si>
+  <si>
+    <t>wet.wt</t>
+  </si>
+  <si>
+    <t>dry.wt</t>
+  </si>
+  <si>
+    <t>day.in</t>
+  </si>
+  <si>
+    <t>day.out</t>
+  </si>
+  <si>
+    <t>total.hrs</t>
+  </si>
+  <si>
+    <t>PRUPEN_SH12</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>16.FEB</t>
+  </si>
+  <si>
+    <t>time.in</t>
+  </si>
+  <si>
+    <t>time.out</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -4188,10 +4226,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4541,6 +4579,40 @@
         <v>10</v>
       </c>
       <c r="G15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4728,4 +4800,408 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="C2">
+        <v>10.879</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>9.6039999999999992</v>
+      </c>
+      <c r="E2">
+        <v>10.4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="C3">
+        <v>13.202</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="0">C3-B3</f>
+        <v>11.920999999999999</v>
+      </c>
+      <c r="E3">
+        <v>10.9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="C4">
+        <v>13.17</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>11.891</v>
+      </c>
+      <c r="E4">
+        <v>10.7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="C5">
+        <v>12.185</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>10.892000000000001</v>
+      </c>
+      <c r="E5">
+        <v>11.3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>1.282</v>
+      </c>
+      <c r="C6">
+        <v>15.253</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>13.971</v>
+      </c>
+      <c r="E6">
+        <v>10.3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="C7">
+        <v>14.895</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>13.606</v>
+      </c>
+      <c r="E7">
+        <v>10.8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="C8">
+        <v>12.282</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>10.977</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>1.284</v>
+      </c>
+      <c r="C9">
+        <v>10.747</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>9.4629999999999992</v>
+      </c>
+      <c r="E9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="C10">
+        <v>11.776</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>10.500999999999999</v>
+      </c>
+      <c r="E10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11">
+        <v>1.282</v>
+      </c>
+      <c r="C11">
+        <v>12.911</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>11.629</v>
+      </c>
+      <c r="E11">
+        <v>11.5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
soil weights... need to work on
</commit_message>
<xml_diff>
--- a/data/treatmentC.xlsx
+++ b/data/treatmentC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="3620" windowWidth="36680" windowHeight="22120" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="24760" yWindow="2720" windowWidth="36680" windowHeight="22120" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">FRZ!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TX.csv!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="259">
   <si>
     <t>OLD</t>
   </si>
@@ -808,6 +808,12 @@
   </si>
   <si>
     <t>time.out</t>
+  </si>
+  <si>
+    <t>20.FEB</t>
+  </si>
+  <si>
+    <t>percent</t>
   </si>
 </sst>
 </file>
@@ -4804,15 +4810,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>210</v>
       </c>
@@ -4846,8 +4852,11 @@
       <c r="K1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -4864,14 +4873,30 @@
       <c r="E2">
         <v>10.4</v>
       </c>
+      <c r="F2">
+        <v>4.0374999999999996</v>
+      </c>
       <c r="G2" t="s">
         <v>254</v>
       </c>
       <c r="H2" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K2">
+        <v>95.5</v>
+      </c>
+      <c r="L2">
+        <f>((C2-F2)/C2)*100</f>
+        <v>62.887213898336249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4888,14 +4913,30 @@
       <c r="E3">
         <v>10.9</v>
       </c>
+      <c r="F3">
+        <v>4.4884000000000004</v>
+      </c>
       <c r="G3" t="s">
         <v>254</v>
       </c>
       <c r="H3" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K3">
+        <v>95.5</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L11" si="1">((C3-F3)/C3)*100</f>
+        <v>66.002120890774123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -4912,14 +4953,30 @@
       <c r="E4">
         <v>10.7</v>
       </c>
+      <c r="F4">
+        <v>4.6595000000000004</v>
+      </c>
       <c r="G4" t="s">
         <v>254</v>
       </c>
       <c r="H4" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>257</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K4">
+        <v>95.5</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>64.620349278663639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -4936,14 +4993,30 @@
       <c r="E5">
         <v>11.3</v>
       </c>
+      <c r="F5">
+        <v>4.4255000000000004</v>
+      </c>
       <c r="G5" t="s">
         <v>254</v>
       </c>
       <c r="H5" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K5">
+        <v>95.5</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>63.680755026672131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -4960,14 +5033,30 @@
       <c r="E6">
         <v>10.3</v>
       </c>
+      <c r="F6">
+        <v>4.9896000000000003</v>
+      </c>
       <c r="G6" t="s">
         <v>254</v>
       </c>
       <c r="H6" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>257</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K6">
+        <v>95.5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>67.287746672785687</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -4984,14 +5073,30 @@
       <c r="E7">
         <v>10.8</v>
       </c>
+      <c r="F7">
+        <v>5.0781999999999998</v>
+      </c>
       <c r="G7" t="s">
         <v>254</v>
       </c>
       <c r="H7" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>257</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K7">
+        <v>95.5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>65.90668009399127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -5008,14 +5113,30 @@
       <c r="E8">
         <v>9</v>
       </c>
+      <c r="F8">
+        <v>4.6997999999999998</v>
+      </c>
       <c r="G8" t="s">
         <v>254</v>
       </c>
       <c r="H8" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>257</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K8">
+        <v>95.5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>61.734245236932097</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -5032,14 +5153,30 @@
       <c r="E9">
         <v>8.6999999999999993</v>
       </c>
+      <c r="F9">
+        <v>4.5034999999999998</v>
+      </c>
       <c r="G9" t="s">
         <v>254</v>
       </c>
       <c r="H9" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K9">
+        <v>95.5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>58.095282404391924</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -5056,14 +5193,30 @@
       <c r="E10">
         <v>10.199999999999999</v>
       </c>
+      <c r="F10">
+        <v>4.4480000000000004</v>
+      </c>
       <c r="G10" t="s">
         <v>254</v>
       </c>
       <c r="H10" s="3">
         <v>0.47916666666666669</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>257</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K10">
+        <v>95.5</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>62.228260869565212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>251</v>
       </c>
@@ -5080,11 +5233,27 @@
       <c r="E11">
         <v>11.5</v>
       </c>
+      <c r="F11">
+        <v>4.7872000000000003</v>
+      </c>
       <c r="G11" t="s">
         <v>254</v>
       </c>
       <c r="H11" s="3">
         <v>0.47916666666666669</v>
+      </c>
+      <c r="I11" t="s">
+        <v>257</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K11">
+        <v>95.5</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>62.921539772287197</v>
       </c>
     </row>
   </sheetData>
@@ -5096,7 +5265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new plants and soil moisture
</commit_message>
<xml_diff>
--- a/data/treatmentC.xlsx
+++ b/data/treatmentC.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="346">
   <si>
     <t>OLD</t>
   </si>
@@ -955,9 +955,6 @@
     <t>SAMRAC_G09</t>
   </si>
   <si>
-    <t>SAMRAC_G010</t>
-  </si>
-  <si>
     <t>SAMRAC_G11</t>
   </si>
   <si>
@@ -1076,6 +1073,9 @@
   </si>
   <si>
     <t>BETPOP_W17</t>
+  </si>
+  <si>
+    <t>SAMRAC_G10</t>
   </si>
 </sst>
 </file>
@@ -6803,15 +6803,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C49"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -6821,8 +6828,23 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -6833,7 +6855,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -6844,7 +6866,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -6855,7 +6877,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>293</v>
       </c>
@@ -6866,7 +6888,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -6877,7 +6899,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -6888,7 +6910,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -6899,7 +6921,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -6910,7 +6932,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -6921,67 +6943,67 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>305</v>
+        <v>345</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>294</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>295</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C16" t="s">
         <v>91</v>
@@ -6992,7 +7014,7 @@
         <v>295</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
@@ -7003,7 +7025,7 @@
         <v>295</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -7014,7 +7036,7 @@
         <v>295</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -7022,10 +7044,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C20" t="s">
         <v>87</v>
@@ -7033,10 +7055,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C21" t="s">
         <v>87</v>
@@ -7044,10 +7066,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -7055,10 +7077,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C23" t="s">
         <v>87</v>
@@ -7066,10 +7088,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
@@ -7077,10 +7099,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C25" t="s">
         <v>87</v>
@@ -7088,10 +7110,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C26" t="s">
         <v>87</v>
@@ -7099,10 +7121,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C27" t="s">
         <v>91</v>
@@ -7110,10 +7132,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C28" t="s">
         <v>91</v>
@@ -7121,10 +7143,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C29" t="s">
         <v>91</v>
@@ -7132,10 +7154,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
@@ -7143,10 +7165,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C31" t="s">
         <v>91</v>
@@ -7154,10 +7176,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C32" t="s">
         <v>91</v>
@@ -7165,10 +7187,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C33" t="s">
         <v>91</v>
@@ -7176,10 +7198,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C34" t="s">
         <v>87</v>
@@ -7187,10 +7209,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C35" t="s">
         <v>87</v>
@@ -7198,10 +7220,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C36" t="s">
         <v>87</v>
@@ -7209,7 +7231,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>143</v>
@@ -7220,10 +7242,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C38" t="s">
         <v>87</v>
@@ -7231,10 +7253,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C39" t="s">
         <v>87</v>
@@ -7242,10 +7264,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C40" t="s">
         <v>87</v>
@@ -7253,10 +7275,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C41" t="s">
         <v>87</v>
@@ -7264,10 +7286,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C42" t="s">
         <v>91</v>
@@ -7275,10 +7297,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C43" t="s">
         <v>91</v>
@@ -7286,10 +7308,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C44" t="s">
         <v>91</v>
@@ -7297,7 +7319,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>155</v>
@@ -7308,10 +7330,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C46" t="s">
         <v>91</v>
@@ -7319,10 +7341,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C47" t="s">
         <v>91</v>
@@ -7330,10 +7352,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C48" t="s">
         <v>91</v>
@@ -7341,7 +7363,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>46</v>
@@ -7351,7 +7373,10 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="85" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added data and meta data for excel sheet
</commit_message>
<xml_diff>
--- a/data/treatmentC.xlsx
+++ b/data/treatmentC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="2300" windowWidth="36680" windowHeight="22120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9400" yWindow="2300" windowWidth="36680" windowHeight="22120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="438">
   <si>
     <t>OLD</t>
   </si>
@@ -1260,6 +1260,99 @@
   </si>
   <si>
     <t>21.MAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBCH </t>
+  </si>
+  <si>
+    <t>MAR.23</t>
+  </si>
+  <si>
+    <t>23.MAR</t>
+  </si>
+  <si>
+    <t>TABS</t>
+  </si>
+  <si>
+    <t>BBCH observations for all individuals through leaf out, once the individual is past leaf out then they were no longer monitored</t>
+  </si>
+  <si>
+    <t>analysis</t>
+  </si>
+  <si>
+    <t>sheet that was synthesized to be converted to a csv for R</t>
+  </si>
+  <si>
+    <t>FRZ</t>
+  </si>
+  <si>
+    <t>all individuals that were put in the growth chamber, with stage, treatment code, time and date</t>
+  </si>
+  <si>
+    <t>tx.counts</t>
+  </si>
+  <si>
+    <t>number of individuals per species per site per treatment - breakdown</t>
+  </si>
+  <si>
+    <t>soil.moisture</t>
+  </si>
+  <si>
+    <t>wet weight and dry weights of soils for 12 individuals over the course of the experiment to test soil moisture</t>
+  </si>
+  <si>
+    <t>NEW.EXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newly added individuals from greenhouse 7 to make data more robust and have less confounding variables. </t>
+  </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>individuals that early signs of struggle</t>
+  </si>
+  <si>
+    <t>GH</t>
+  </si>
+  <si>
+    <t>greenhouse temperature and humidity</t>
+  </si>
+  <si>
+    <t>old ID name and number</t>
+  </si>
+  <si>
+    <t>new experimental ID</t>
+  </si>
+  <si>
+    <t>is the treatment code associated with individual</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>is the soil moisture meter reading and date</t>
+  </si>
+  <si>
+    <t>is the BBCH stage individual is at on that date</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>columns that have been watered that day</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>rows of individuals that have been in the growth chamber</t>
+  </si>
+  <si>
+    <t>Double Frost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New sheet: need to determine which individuals should receive a second frost event. Will try before leaf out and after leaf out. </t>
   </si>
 </sst>
 </file>
@@ -1669,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,8 +1882,149 @@
         <v>277</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>412</v>
+      </c>
+      <c r="B27" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>414</v>
+      </c>
+      <c r="B28" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>416</v>
+      </c>
+      <c r="B29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>418</v>
+      </c>
+      <c r="B30" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>420</v>
+      </c>
+      <c r="B31" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>422</v>
+      </c>
+      <c r="B32" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>424</v>
+      </c>
+      <c r="B33" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>429</v>
+      </c>
+      <c r="B39" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>432</v>
+      </c>
+      <c r="B42" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>434</v>
+      </c>
+      <c r="B43" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>437</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1799,11 +2033,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R149"/>
+  <dimension ref="A1:V149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R39" sqref="R39"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1812,9 +2046,10 @@
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1869,8 +2104,20 @@
       <c r="R1" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>407</v>
+      </c>
+      <c r="T1" t="s">
+        <v>211</v>
+      </c>
+      <c r="U1" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +2156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1948,7 +2195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1973,7 +2220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2006,7 +2253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2056,7 +2303,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -2086,7 +2333,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2120,7 +2367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -2154,7 +2401,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2185,7 +2432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2219,7 +2466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2253,7 +2500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2284,7 +2531,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2306,7 +2553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -4244,6 +4491,9 @@
       <c r="Q78" s="1" t="s">
         <v>383</v>
       </c>
+      <c r="R78" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -4283,6 +4533,9 @@
       <c r="Q79" s="1" t="s">
         <v>383</v>
       </c>
+      <c r="R79" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
@@ -4317,8 +4570,11 @@
         <v>383</v>
       </c>
       <c r="Q80" s="1"/>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R80" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -4351,8 +4607,11 @@
         <v>383</v>
       </c>
       <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R81" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>52</v>
       </c>
@@ -4393,8 +4652,11 @@
         <v>369</v>
       </c>
       <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R82" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>43</v>
       </c>
@@ -4427,8 +4689,11 @@
         <v>383</v>
       </c>
       <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R83" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>139</v>
       </c>
@@ -4460,8 +4725,11 @@
       <c r="N84" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R84" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>144</v>
       </c>
@@ -4490,8 +4758,11 @@
       <c r="N85" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R85" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>43</v>
       </c>
@@ -4523,8 +4794,11 @@
       <c r="N86" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R86" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>142</v>
       </c>
@@ -4559,8 +4833,11 @@
       <c r="N87" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R87" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -4595,8 +4872,11 @@
       <c r="N88" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R88" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>162</v>
       </c>
@@ -4630,8 +4910,11 @@
       <c r="N89" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R89" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>162</v>
       </c>
@@ -4665,8 +4948,11 @@
       <c r="O90" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R90" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>61</v>
       </c>
@@ -4700,8 +4986,11 @@
       <c r="N91" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>61</v>
       </c>
@@ -4743,8 +5032,11 @@
         <v>369</v>
       </c>
       <c r="Q92" s="1"/>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R92" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>57</v>
       </c>
@@ -4783,8 +5075,11 @@
         <v>383</v>
       </c>
       <c r="Q93" s="1"/>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R93" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>73</v>
       </c>
@@ -4823,8 +5118,11 @@
         <v>369</v>
       </c>
       <c r="Q94" s="1"/>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R94" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>170</v>
       </c>
@@ -4856,8 +5154,11 @@
       <c r="N95" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R95" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>78</v>
       </c>
@@ -4892,8 +5193,11 @@
       <c r="N96" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R96" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>70</v>
       </c>
@@ -4930,8 +5234,11 @@
       <c r="N97" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R97" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>177</v>
       </c>
@@ -4968,8 +5275,11 @@
       <c r="N98" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R98" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>70</v>
       </c>
@@ -5006,8 +5316,11 @@
       <c r="N99" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R99" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>70</v>
       </c>
@@ -5047,8 +5360,11 @@
       <c r="N100" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R100" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>177</v>
       </c>
@@ -5077,8 +5393,11 @@
       <c r="N101" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R101" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>177</v>
       </c>
@@ -5113,8 +5432,11 @@
       <c r="N102" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R102" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>73</v>
       </c>
@@ -5151,8 +5473,11 @@
       <c r="N103" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R103" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>73</v>
       </c>
@@ -5189,8 +5514,11 @@
       <c r="N104" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R104" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>73</v>
       </c>
@@ -5227,8 +5555,11 @@
       <c r="N105" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R105" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>76</v>
       </c>
@@ -5260,8 +5591,11 @@
       <c r="N106" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R106" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>76</v>
       </c>
@@ -5298,8 +5632,11 @@
       <c r="N107" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R107" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>66</v>
       </c>
@@ -5333,8 +5670,11 @@
       <c r="N108" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R108" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>66</v>
       </c>
@@ -5371,8 +5711,11 @@
       <c r="N109" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R109" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>66</v>
       </c>
@@ -5406,8 +5749,11 @@
       <c r="N110" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R110" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>23</v>
       </c>
@@ -5442,8 +5788,11 @@
       <c r="Q111" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R111" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>14</v>
       </c>
@@ -5477,6 +5826,9 @@
       </c>
       <c r="Q112" s="1" t="s">
         <v>377</v>
+      </c>
+      <c r="R112" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
@@ -5518,6 +5870,9 @@
         <v>377</v>
       </c>
       <c r="Q113" s="1"/>
+      <c r="R113" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
@@ -5558,6 +5913,9 @@
         <v>377</v>
       </c>
       <c r="Q114" s="1"/>
+      <c r="R114" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
@@ -5595,6 +5953,9 @@
         <v>369</v>
       </c>
       <c r="Q115" s="1"/>
+      <c r="R115" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
@@ -5643,6 +6004,9 @@
         <v>369</v>
       </c>
       <c r="Q116" s="1"/>
+      <c r="R116" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
@@ -5681,8 +6045,8 @@
       <c r="N117" t="s">
         <v>370</v>
       </c>
-      <c r="R117">
-        <v>15</v>
+      <c r="R117" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
@@ -5719,6 +6083,9 @@
       <c r="N118" t="s">
         <v>370</v>
       </c>
+      <c r="R118" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
@@ -5755,6 +6122,9 @@
       <c r="N119" t="s">
         <v>371</v>
       </c>
+      <c r="R119" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
@@ -5805,6 +6175,9 @@
       <c r="Q120" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="R120" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
@@ -5843,6 +6216,9 @@
       <c r="N121" t="s">
         <v>370</v>
       </c>
+      <c r="R121" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
@@ -5879,6 +6255,9 @@
       <c r="N122" t="s">
         <v>370</v>
       </c>
+      <c r="R122" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
@@ -5912,6 +6291,9 @@
       <c r="N123" t="s">
         <v>373</v>
       </c>
+      <c r="R123" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
@@ -5951,6 +6333,9 @@
       <c r="N124" t="s">
         <v>375</v>
       </c>
+      <c r="R124" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
@@ -5987,6 +6372,9 @@
       <c r="N125" t="s">
         <v>373</v>
       </c>
+      <c r="R125" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
@@ -6020,6 +6408,9 @@
       <c r="N126" t="s">
         <v>376</v>
       </c>
+      <c r="R126" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
@@ -6053,6 +6444,9 @@
       <c r="N127" t="s">
         <v>354</v>
       </c>
+      <c r="R127" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
@@ -6091,8 +6485,11 @@
       <c r="N128" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R128" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>73</v>
       </c>
@@ -6132,8 +6529,11 @@
       <c r="N129" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R129" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>195</v>
       </c>
@@ -6168,8 +6568,11 @@
       <c r="N130" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R130" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>66</v>
       </c>
@@ -6204,8 +6607,11 @@
       <c r="N131" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R131" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>195</v>
       </c>
@@ -6237,8 +6643,11 @@
       <c r="N132" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R132" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>78</v>
       </c>
@@ -6280,8 +6689,11 @@
         <v>369</v>
       </c>
       <c r="Q133" s="1"/>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R133" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>70</v>
       </c>
@@ -6322,8 +6734,11 @@
         <v>369</v>
       </c>
       <c r="Q134" s="1"/>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R134" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>67</v>
       </c>
@@ -6365,8 +6780,11 @@
         <v>369</v>
       </c>
       <c r="Q135" s="1"/>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R135" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>73</v>
       </c>
@@ -6402,8 +6820,11 @@
         <v>369</v>
       </c>
       <c r="Q136" s="1"/>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R136" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>83</v>
       </c>
@@ -6447,8 +6868,11 @@
       <c r="Q137" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R137" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>66</v>
       </c>
@@ -6493,8 +6917,11 @@
         <v>377</v>
       </c>
       <c r="Q138" s="1"/>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R138" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>21</v>
       </c>
@@ -6531,8 +6958,11 @@
       <c r="P139" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R139" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>49</v>
       </c>
@@ -6569,8 +6999,11 @@
       <c r="P140" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R140" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>43</v>
       </c>
@@ -6598,8 +7031,11 @@
       <c r="N141" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R141" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>43</v>
       </c>
@@ -6642,8 +7078,11 @@
       <c r="P142" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R142" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>45</v>
       </c>
@@ -6689,8 +7128,11 @@
       <c r="Q143" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R143" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>43</v>
       </c>
@@ -6727,8 +7169,11 @@
       <c r="N144" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R144" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>43</v>
       </c>
@@ -6768,8 +7213,11 @@
       <c r="N145" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R145" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>78</v>
       </c>
@@ -6803,8 +7251,11 @@
       <c r="N146" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R146" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>78</v>
       </c>
@@ -6841,8 +7292,11 @@
       <c r="N147" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R147" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>78</v>
       </c>
@@ -6873,8 +7327,11 @@
       <c r="N148" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R148" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>78</v>
       </c>
@@ -6904,6 +7361,9 @@
       </c>
       <c r="N149" t="s">
         <v>380</v>
+      </c>
+      <c r="R149" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -6911,7 +7371,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="99" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="34" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -10534,10 +10994,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12151,6 +12611,74 @@
       </c>
       <c r="H64" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" t="s">
+        <v>409</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="F65">
+        <v>12</v>
+      </c>
+      <c r="G65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>409</v>
+      </c>
+      <c r="C66" s="3">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="F66">
+        <v>12</v>
+      </c>
+      <c r="G66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>409</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="F67">
+        <v>12</v>
+      </c>
+      <c r="G67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" t="s">
+        <v>409</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="F68">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -12336,20 +12864,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -12393,7 +12926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -12436,7 +12969,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -12479,7 +13012,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -12522,7 +13055,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -12565,7 +13098,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -12608,7 +13141,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -12651,7 +13184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -12694,7 +13227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -12737,7 +13270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -12780,7 +13313,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -12823,7 +13356,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -12863,7 +13396,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -12903,7 +13436,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>178</v>
       </c>
@@ -12943,7 +13476,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -12983,7 +13516,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -13023,7 +13556,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>199</v>
       </c>
@@ -13063,7 +13596,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -13103,7 +13636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -13143,7 +13676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -13183,7 +13716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -13223,7 +13756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -13256,7 +13789,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>131</v>
       </c>
@@ -13289,7 +13822,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -13322,7 +13855,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>160</v>
       </c>
@@ -13355,7 +13888,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -13388,7 +13921,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -13421,7 +13954,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -13454,7 +13987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -13487,7 +14020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -13520,7 +14053,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -13553,7 +14086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -13586,7 +14119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -13619,7 +14152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -13652,7 +14185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -13685,7 +14218,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>178</v>
       </c>
@@ -13718,7 +14251,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -13751,7 +14284,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -13784,7 +14317,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>199</v>
       </c>
@@ -13817,7 +14350,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -13850,7 +14383,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -13883,7 +14416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -13916,7 +14449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -13949,7 +14482,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -13982,7 +14515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -14015,8 +14548,239 @@
         <v>5</v>
       </c>
     </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46">
+        <v>11.771000000000001</v>
+      </c>
+      <c r="G46" t="s">
+        <v>408</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47">
+        <v>12.689</v>
+      </c>
+      <c r="G47" t="s">
+        <v>408</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48">
+        <v>10.932</v>
+      </c>
+      <c r="G48" t="s">
+        <v>408</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49">
+        <v>12.311999999999999</v>
+      </c>
+      <c r="G49" t="s">
+        <v>408</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50">
+        <v>10.342000000000001</v>
+      </c>
+      <c r="G50" t="s">
+        <v>408</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51">
+        <v>9.66</v>
+      </c>
+      <c r="G51" t="s">
+        <v>408</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>10.509</v>
+      </c>
+      <c r="G52" t="s">
+        <v>408</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53">
+        <v>9.8219999999999992</v>
+      </c>
+      <c r="G53" t="s">
+        <v>408</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54">
+        <v>12.757999999999999</v>
+      </c>
+      <c r="G54" t="s">
+        <v>408</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55">
+        <v>10.352</v>
+      </c>
+      <c r="G55" t="s">
+        <v>408</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56">
+        <v>11.042</v>
+      </c>
+      <c r="G56" t="s">
+        <v>408</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57">
+        <v>11.2074</v>
+      </c>
+      <c r="G57" t="s">
+        <v>408</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="92" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -15362,5 +16126,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>